<commit_message>
Async Await Working Sample
</commit_message>
<xml_diff>
--- a/C#/Refresher.xlsx
+++ b/C#/Refresher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\all-languages\C#\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6598218-4D15-481C-9E8F-D67272AE1EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3399F7-42C0-4928-BC74-33C269DE6507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>We cannot just put C# code into a file and expect an operating system or a CPU to understand the instructions inside. There has to be a</t>
   </si>
@@ -159,6 +159,15 @@
       </rPr>
       <t xml:space="preserve"> feature. </t>
     </r>
+  </si>
+  <si>
+    <t>WHAT IS A CLASS</t>
+  </si>
+  <si>
+    <t>Class is a type, which we can use to do some work and it also stores some data.</t>
+  </si>
+  <si>
+    <t>In software, we are trying to build the right abstraction and have proper encapsulation and build the right model to manage the complexity</t>
   </si>
 </sst>
 </file>
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C25"/>
+  <dimension ref="B1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,6 +632,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>